<commit_message>
Analisis parte como 3 porque ya perdi la cuenta
Si
</commit_message>
<xml_diff>
--- a/ANALISIS PRACTICA 2.xlsx
+++ b/ANALISIS PRACTICA 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\Documents\C4\Algoritmos Clasicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B8B212-6E1F-40D8-A9F5-03724E9E84BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE4030D-9ABA-41DA-A825-A7953B5648AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F1160D50-0CF7-4668-94EF-40E3F0C29523}"/>
   </bookViews>
@@ -271,13 +271,13 @@
                   <c:v>4600</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>142500</c:v>
+                  <c:v>122500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2643300</c:v>
+                  <c:v>1741300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34079800</c:v>
+                  <c:v>29079800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1824,13 +1824,13 @@
                   <c:v>174100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1745900</c:v>
+                  <c:v>1145900</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7296900</c:v>
+                  <c:v>3296900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32168300</c:v>
+                  <c:v>29168300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4934,8 +4934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116D027C-5E57-4F97-8AF3-F3D772021D4F}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="108" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5023,7 +5023,7 @@
         <v>39556.788426515748</v>
       </c>
       <c r="D4" s="1">
-        <v>142500</v>
+        <v>122500</v>
       </c>
       <c r="G4" s="1">
         <v>100</v>
@@ -5033,7 +5033,7 @@
         <v>200</v>
       </c>
       <c r="I4" s="1">
-        <v>1745900</v>
+        <v>1145900</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -5049,7 +5049,7 @@
         <v>5993565.9227377558</v>
       </c>
       <c r="D5" s="1">
-        <v>2643300</v>
+        <v>1741300</v>
       </c>
       <c r="G5" s="1">
         <v>1000</v>
@@ -5059,7 +5059,7 @@
         <v>2999.9999999999995</v>
       </c>
       <c r="I5" s="1">
-        <v>7296900</v>
+        <v>3296900</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -5075,7 +5075,7 @@
         <v>799915657.27233553</v>
       </c>
       <c r="D6" s="1">
-        <v>34079800</v>
+        <v>29079800</v>
       </c>
       <c r="G6" s="1">
         <v>10000</v>
@@ -5085,7 +5085,7 @@
         <v>40000</v>
       </c>
       <c r="I6" s="1">
-        <v>32168300</v>
+        <v>29168300</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>